<commit_message>
added detail to in-progress functions
</commit_message>
<xml_diff>
--- a/FunctionList.xlsx
+++ b/FunctionList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tombannerman/Documents/GitHub/flightmechASS3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamh\Documents\UNI\Y4S2\AERO3560\A3\flightmechASS3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C152C55-CA9D-F341-BBE2-CF2FC88DD8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C125D39-AF49-4BBD-98FC-2B201E412685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{24E78D1A-753C-6B44-A1DE-CCBCD617B7D0}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{24E78D1A-753C-6B44-A1DE-CCBCD617B7D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Initialisation.m</t>
   </si>
@@ -115,6 +115,30 @@
   </si>
   <si>
     <t>Output: eg [c, d] c: 1x9, d: 1x4</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Aircraft object</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Flight plan (int), time (float)</t>
+  </si>
+  <si>
+    <t>Controls delta_T, delta_e, delta_a, delta_r</t>
+  </si>
+  <si>
+    <t>Main structure done but need to add actual flight plans</t>
+  </si>
+  <si>
+    <t>Quaternions (4xn, float)</t>
+  </si>
+  <si>
+    <t>Euler angles (3xn, rads)</t>
   </si>
 </sst>
 </file>
@@ -155,9 +179,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,15 +499,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30562038-A4C2-4F48-B27F-09A880394B18}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.70703125" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
@@ -516,6 +541,18 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
@@ -536,6 +573,21 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
@@ -581,35 +633,71 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added flow properties function
</commit_message>
<xml_diff>
--- a/FunctionList.xlsx
+++ b/FunctionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamh\Documents\UNI\Y4S2\AERO3560\A3\flightmechASS3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C125D39-AF49-4BBD-98FC-2B201E412685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11FE39E-9017-4BE2-8B4E-ED04326E8E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{24E78D1A-753C-6B44-A1DE-CCBCD617B7D0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>Initialisation.m</t>
   </si>
@@ -139,6 +139,21 @@
   </si>
   <si>
     <t>Euler angles (3xn, rads)</t>
+  </si>
+  <si>
+    <t>angle (rads)</t>
+  </si>
+  <si>
+    <t>3x3 (float)</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>state vector</t>
+  </si>
+  <si>
+    <t>trim inputs</t>
   </si>
 </sst>
 </file>
@@ -500,7 +515,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -558,6 +573,18 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
@@ -613,6 +640,9 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
@@ -650,15 +680,51 @@
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6">

</xml_diff>